<commit_message>
updating excell sheet creation
</commit_message>
<xml_diff>
--- a/src/test/resources/excelSheet/vipinproject.xlsx
+++ b/src/test/resources/excelSheet/vipinproject.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vipin\eclipse-workspace\POM_project\src\test\resources\excelSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vipin\eclipse-workspace\POM_project_end_to_end_Runner_XYZBANKProcess\src\test\resources\excelSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784224C1-EAF7-45E3-815B-667CEDBD8768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C5C6B2-6352-4A3E-82EE-1318C0573532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="2112" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Service</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -361,7 +358,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>